<commit_message>
Update Mini Project Product Backlog.xlsx
</commit_message>
<xml_diff>
--- a/Documenten/Mini Project Product Backlog.xlsx
+++ b/Documenten/Mini Project Product Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amzir\Documents\GitHub\Mini-Project\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F687A624-4982-46BF-90D2-341992AEF3F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE420A2-FAEA-4A81-8087-AE31A0239086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Alihan</t>
+  </si>
+  <si>
+    <t>Adel</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -712,7 +715,9 @@
       <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19">
@@ -724,7 +729,9 @@
       <c r="C4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
@@ -751,7 +758,9 @@
       <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -777,7 +786,9 @@
       <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -820,6 +831,9 @@
       <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -832,7 +846,9 @@
       <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="17" t="s">
+        <v>41</v>
+      </c>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -845,7 +861,9 @@
       <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,7 +921,9 @@
       <c r="C17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -916,7 +936,9 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -941,7 +963,9 @@
       <c r="C20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="17"/>
+      <c r="D20" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -969,7 +993,9 @@
       <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3174,6 +3200,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010065DA0B4C524F55429CE2FD5B93B01F74" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0b81802aa35bff97fe2d4068698eefb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ea016a50-4395-487d-ae85-89d5607ff42b" xmlns:ns3="1f7ab50f-86ca-4990-8cf2-d29dc34c52f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b03203aba3005218e1fa3e02034dd03" ns2:_="" ns3:_="">
     <xsd:import namespace="ea016a50-4395-487d-ae85-89d5607ff42b"/>
@@ -3338,22 +3379,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C084766E-1400-4040-81BA-5DFB82754CBA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E847B739-67F9-4ADE-9E6F-0F08F6F51A70}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52455CA5-ED3E-453B-9081-F967EEE159E1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3370,21 +3413,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E847B739-67F9-4ADE-9E6F-0F08F6F51A70}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C084766E-1400-4040-81BA-5DFB82754CBA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>